<commit_message>
additional emails for multicountry
</commit_message>
<xml_diff>
--- a/xlsx_files/ati_multicountry_emails_04.12.2023 (not complete).xlsx
+++ b/xlsx_files/ati_multicountry_emails_04.12.2023 (not complete).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Job\Prometeo\ati.su\xlsx_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2915A8E-D137-49D1-8EB1-2E01ACE83568}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1AE50FA-CB85-4ABE-ABA8-AA1B1127E007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30033,10 +30033,10 @@
   <dimension ref="A1:F3414"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2422" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B3395" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E2427" sqref="E2427"/>
+      <selection pane="bottomRight" activeCell="E3411" sqref="E3411"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>